<commit_message>
Biomass and catch removed 20 yrs burn in
</commit_message>
<xml_diff>
--- a/noba_simdata/Catch.xlsx
+++ b/noba_simdata/Catch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Howard.Townsend\Documents\EM Toolbox\MSSPM Projects\MSSPM-Keyruns\noba_simdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94984956-C1ED-4F7D-AA5A-F579D9A92FC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3D207098-8F70-4E83-ACD1-6DC939B3A40B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
@@ -539,8 +539,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -898,13 +899,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L145" sqref="B22:L145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -980,7 +981,7 @@
         <v>204.84717591056901</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1018,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1056,7 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1094,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1246,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1284,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1322,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1360,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1436,7 +1437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1510,12 +1511,6 @@
       </c>
       <c r="L16">
         <v>2599732.9387959102</v>
-      </c>
-      <c r="N16">
-        <v>1</v>
-      </c>
-      <c r="O16">
-        <v>1891</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1555,12 +1550,6 @@
       <c r="L17">
         <v>2206162.82239928</v>
       </c>
-      <c r="N17">
-        <v>2</v>
-      </c>
-      <c r="O17">
-        <v>1892</v>
-      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1599,12 +1588,6 @@
       <c r="L18">
         <v>1818121.4069164901</v>
       </c>
-      <c r="N18">
-        <v>3</v>
-      </c>
-      <c r="O18">
-        <v>1893</v>
-      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1643,12 +1626,6 @@
       <c r="L19">
         <v>1523522.7314876399</v>
       </c>
-      <c r="N19">
-        <v>4</v>
-      </c>
-      <c r="O19">
-        <v>1894</v>
-      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1687,12 +1664,6 @@
       <c r="L20">
         <v>1260859.96322954</v>
       </c>
-      <c r="N20">
-        <v>5</v>
-      </c>
-      <c r="O20">
-        <v>1895</v>
-      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1731,55 +1702,49 @@
       <c r="L21">
         <v>1085082.4987627</v>
       </c>
-      <c r="N21">
-        <v>6</v>
-      </c>
-      <c r="O21">
-        <v>1896</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22">
+    </row>
+    <row r="22" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>1080462.5852138</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>454789.104509742</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>20703.186907134499</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>29559.675172404801</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
         <v>203680.96397593501</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="1">
         <v>1892795.5577098499</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="1">
         <v>21985.365799620598</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
         <v>68958.826813485095</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="1">
         <v>919151.92870750395</v>
       </c>
-      <c r="N22">
-        <v>7</v>
-      </c>
-      <c r="O22">
-        <v>1897</v>
+      <c r="N22" s="1">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1">
+        <v>1891</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1820,10 +1785,10 @@
         <v>769977.06126921403</v>
       </c>
       <c r="N23">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="O23">
-        <v>1898</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1864,10 +1829,10 @@
         <v>640978.89758427802</v>
       </c>
       <c r="N24">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="O24">
-        <v>1899</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -1908,10 +1873,10 @@
         <v>531937.03217438899</v>
       </c>
       <c r="N25">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="O25">
-        <v>1900</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1952,10 +1917,10 @@
         <v>662963.36852546898</v>
       </c>
       <c r="N26">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="O26">
-        <v>1901</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -1996,10 +1961,10 @@
         <v>515273.33707567002</v>
       </c>
       <c r="N27">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="O27">
-        <v>1902</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2039,11 +2004,11 @@
       <c r="L28">
         <v>370725.13725165598</v>
       </c>
-      <c r="N28">
-        <v>13</v>
-      </c>
-      <c r="O28">
-        <v>1903</v>
+      <c r="N28" s="1">
+        <v>7</v>
+      </c>
+      <c r="O28" s="1">
+        <v>1897</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2084,10 +2049,10 @@
         <v>357250.12406964798</v>
       </c>
       <c r="N29">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="O29">
-        <v>1904</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -2128,10 +2093,10 @@
         <v>217776.416400146</v>
       </c>
       <c r="N30">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="O30">
-        <v>1905</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -2172,10 +2137,10 @@
         <v>125572.059614474</v>
       </c>
       <c r="N31">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="O31">
-        <v>1906</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -2216,10 +2181,10 @@
         <v>154310.03627225599</v>
       </c>
       <c r="N32">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="O32">
-        <v>1907</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2260,10 +2225,10 @@
         <v>162489.57955673899</v>
       </c>
       <c r="N33">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="O33">
-        <v>1908</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -2304,10 +2269,10 @@
         <v>154980.52069477699</v>
       </c>
       <c r="N34">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="O34">
-        <v>1909</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -2348,10 +2313,10 @@
         <v>111211.69182317</v>
       </c>
       <c r="N35">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="O35">
-        <v>1910</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -2392,10 +2357,10 @@
         <v>90545.8780632376</v>
       </c>
       <c r="N36">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="O36">
-        <v>1911</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -2436,10 +2401,10 @@
         <v>80570.695864911904</v>
       </c>
       <c r="N37">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="O37">
-        <v>1912</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -2480,10 +2445,10 @@
         <v>87939.164084429707</v>
       </c>
       <c r="N38">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="O38">
-        <v>1913</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -2524,10 +2489,10 @@
         <v>90978.203406945599</v>
       </c>
       <c r="N39">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="O39">
-        <v>1914</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -2568,10 +2533,10 @@
         <v>87165.086721686806</v>
       </c>
       <c r="N40">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="O40">
-        <v>1915</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -2612,10 +2577,10 @@
         <v>78873.577150911398</v>
       </c>
       <c r="N41">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="O41">
-        <v>1916</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -2656,10 +2621,10 @@
         <v>70537.804618623297</v>
       </c>
       <c r="N42">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="O42">
-        <v>1917</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -2700,10 +2665,10 @@
         <v>74305.789562618302</v>
       </c>
       <c r="N43">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="O43">
-        <v>1918</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -2744,10 +2709,10 @@
         <v>78868.324760069401</v>
       </c>
       <c r="N44">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="O44">
-        <v>1919</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -2788,10 +2753,10 @@
         <v>78886.267969621404</v>
       </c>
       <c r="N45">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="O45">
-        <v>1920</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -2832,10 +2797,10 @@
         <v>82625.8440644605</v>
       </c>
       <c r="N46">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="O46">
-        <v>1921</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -2876,10 +2841,10 @@
         <v>95106.3774592134</v>
       </c>
       <c r="N47">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="O47">
-        <v>1922</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -2920,10 +2885,10 @@
         <v>107824.25729827301</v>
       </c>
       <c r="N48">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="O48">
-        <v>1923</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -2964,10 +2929,10 @@
         <v>116172.93629754</v>
       </c>
       <c r="N49">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="O49">
-        <v>1924</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -3008,10 +2973,10 @@
         <v>126846.816786831</v>
       </c>
       <c r="N50">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="O50">
-        <v>1925</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -3052,10 +3017,10 @@
         <v>177953.785194583</v>
       </c>
       <c r="N51">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="O51">
-        <v>1926</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -3096,10 +3061,10 @@
         <v>178374.611565759</v>
       </c>
       <c r="N52">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="O52">
-        <v>1927</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -3140,10 +3105,10 @@
         <v>192704.604095663</v>
       </c>
       <c r="N53">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="O53">
-        <v>1928</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -3184,10 +3149,10 @@
         <v>183452.12028843601</v>
       </c>
       <c r="N54">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="O54">
-        <v>1929</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -3228,10 +3193,10 @@
         <v>208451.01348777901</v>
       </c>
       <c r="N55">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="O55">
-        <v>1930</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
@@ -3272,10 +3237,10 @@
         <v>194749.17408261701</v>
       </c>
       <c r="N56">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="O56">
-        <v>1931</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -3316,10 +3281,10 @@
         <v>194610.60955714301</v>
       </c>
       <c r="N57">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="O57">
-        <v>1932</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -3360,10 +3325,10 @@
         <v>155580.89622374301</v>
       </c>
       <c r="N58">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="O58">
-        <v>1933</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -3404,10 +3369,10 @@
         <v>151253.46991027199</v>
       </c>
       <c r="N59">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="O59">
-        <v>1934</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -3448,10 +3413,10 @@
         <v>163346.18971405199</v>
       </c>
       <c r="N60">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O60">
-        <v>1935</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -3492,10 +3457,10 @@
         <v>32699.9622608926</v>
       </c>
       <c r="N61">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="O61">
-        <v>1936</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -3536,10 +3501,10 @@
         <v>40185.668664267003</v>
       </c>
       <c r="N62">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="O62">
-        <v>1937</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -3580,10 +3545,10 @@
         <v>48301.243733551397</v>
       </c>
       <c r="N63">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="O63">
-        <v>1938</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -3624,10 +3589,10 @@
         <v>57339.170365207297</v>
       </c>
       <c r="N64">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="O64">
-        <v>1939</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
@@ -3668,10 +3633,10 @@
         <v>68466.800760896105</v>
       </c>
       <c r="N65">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="O65">
-        <v>1940</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
@@ -3712,10 +3677,10 @@
         <v>80196.319232212103</v>
       </c>
       <c r="N66">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="O66">
-        <v>1941</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
@@ -3756,10 +3721,10 @@
         <v>94863.082673821802</v>
       </c>
       <c r="N67">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="O67">
-        <v>1942</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
@@ -3800,10 +3765,10 @@
         <v>109672.477113612</v>
       </c>
       <c r="N68">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="O68">
-        <v>1943</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
@@ -3844,10 +3809,10 @@
         <v>127738.590649994</v>
       </c>
       <c r="N69">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="O69">
-        <v>1944</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
@@ -3888,10 +3853,10 @@
         <v>148571.26428720701</v>
       </c>
       <c r="N70">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="O70">
-        <v>1945</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
@@ -3932,10 +3897,10 @@
         <v>166062.50468408701</v>
       </c>
       <c r="N71">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="O71">
-        <v>1946</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
@@ -3976,10 +3941,10 @@
         <v>192781.32718048099</v>
       </c>
       <c r="N72">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="O72">
-        <v>1947</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
@@ -4020,10 +3985,10 @@
         <v>213581.622837456</v>
       </c>
       <c r="N73">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="O73">
-        <v>1948</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
@@ -4064,10 +4029,10 @@
         <v>245646.674097896</v>
       </c>
       <c r="N74">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="O74">
-        <v>1949</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
@@ -4108,10 +4073,10 @@
         <v>271306.42685422697</v>
       </c>
       <c r="N75">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="O75">
-        <v>1950</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
@@ -4152,10 +4117,10 @@
         <v>299275.09685728198</v>
       </c>
       <c r="N76">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="O76">
-        <v>1951</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
@@ -4196,10 +4161,10 @@
         <v>328928.71764681197</v>
       </c>
       <c r="N77">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="O77">
-        <v>1952</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
@@ -4240,10 +4205,10 @@
         <v>345742.00028462597</v>
       </c>
       <c r="N78">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="O78">
-        <v>1953</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -4284,10 +4249,10 @@
         <v>363226.50783176097</v>
       </c>
       <c r="N79">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="O79">
-        <v>1954</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
@@ -4328,10 +4293,10 @@
         <v>385665.024009271</v>
       </c>
       <c r="N80">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="O80">
-        <v>1955</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
@@ -4372,10 +4337,10 @@
         <v>397628.02979467</v>
       </c>
       <c r="N81">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="O81">
-        <v>1956</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
@@ -4416,10 +4381,10 @@
         <v>413678.078916181</v>
       </c>
       <c r="N82">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="O82">
-        <v>1957</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
@@ -4460,10 +4425,10 @@
         <v>430908.988222079</v>
       </c>
       <c r="N83">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="O83">
-        <v>1958</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
@@ -4504,10 +4469,10 @@
         <v>439408.67190834001</v>
       </c>
       <c r="N84">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="O84">
-        <v>1959</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
@@ -4548,10 +4513,10 @@
         <v>464646.12496131798</v>
       </c>
       <c r="N85">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="O85">
-        <v>1960</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
@@ -4592,10 +4557,10 @@
         <v>481411.63178324298</v>
       </c>
       <c r="N86">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="O86">
-        <v>1961</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
@@ -4636,10 +4601,10 @@
         <v>495923.80144373298</v>
       </c>
       <c r="N87">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="O87">
-        <v>1962</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
@@ -4680,10 +4645,10 @@
         <v>523183.91447213298</v>
       </c>
       <c r="N88">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="O88">
-        <v>1963</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
@@ -4724,10 +4689,10 @@
         <v>532860.18105056603</v>
       </c>
       <c r="N89">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="O89">
-        <v>1964</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
@@ -4768,10 +4733,10 @@
         <v>554405.32109236298</v>
       </c>
       <c r="N90">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="O90">
-        <v>1965</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
@@ -4812,10 +4777,10 @@
         <v>550994.68708585599</v>
       </c>
       <c r="N91">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="O91">
-        <v>1966</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
@@ -4856,10 +4821,10 @@
         <v>562238.03505930502</v>
       </c>
       <c r="N92">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="O92">
-        <v>1967</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
@@ -4900,10 +4865,10 @@
         <v>566686.28565343202</v>
       </c>
       <c r="N93">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="O93">
-        <v>1968</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
@@ -4944,10 +4909,10 @@
         <v>582260.23186869</v>
       </c>
       <c r="N94">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="O94">
-        <v>1969</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
@@ -4988,10 +4953,10 @@
         <v>581516.614521796</v>
       </c>
       <c r="N95">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="O95">
-        <v>1970</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
@@ -5032,10 +4997,10 @@
         <v>582917.782173021</v>
       </c>
       <c r="N96">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="O96">
-        <v>1971</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
@@ -5076,10 +5041,10 @@
         <v>591069.26860139496</v>
       </c>
       <c r="N97">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="O97">
-        <v>1972</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
@@ -5120,10 +5085,10 @@
         <v>589318.948453538</v>
       </c>
       <c r="N98">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="O98">
-        <v>1973</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
@@ -5164,10 +5129,10 @@
         <v>584346.83554578898</v>
       </c>
       <c r="N99">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="O99">
-        <v>1974</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
@@ -5208,10 +5173,10 @@
         <v>593616.51131778001</v>
       </c>
       <c r="N100">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="O100">
-        <v>1975</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -5252,10 +5217,10 @@
         <v>608216.64209593099</v>
       </c>
       <c r="N101">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="O101">
-        <v>1976</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
@@ -5296,10 +5261,10 @@
         <v>607068.53314675495</v>
       </c>
       <c r="N102">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="O102">
-        <v>1977</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -5340,10 +5305,10 @@
         <v>637700.93562895001</v>
       </c>
       <c r="N103">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="O103">
-        <v>1978</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
@@ -5384,10 +5349,10 @@
         <v>626145.75784752402</v>
       </c>
       <c r="N104">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O104">
-        <v>1979</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
@@ -5428,10 +5393,10 @@
         <v>629856.87003970798</v>
       </c>
       <c r="N105">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="O105">
-        <v>1980</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
@@ -5472,10 +5437,10 @@
         <v>638285.35912210704</v>
       </c>
       <c r="N106">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="O106">
-        <v>1981</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
@@ -5516,10 +5481,10 @@
         <v>638896.751580899</v>
       </c>
       <c r="N107">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="O107">
-        <v>1982</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
@@ -5560,10 +5525,10 @@
         <v>628602.27889276901</v>
       </c>
       <c r="N108">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="O108">
-        <v>1983</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
@@ -5604,10 +5569,10 @@
         <v>633381.14181100205</v>
       </c>
       <c r="N109">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="O109">
-        <v>1984</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
@@ -5648,10 +5613,10 @@
         <v>620558.19971818896</v>
       </c>
       <c r="N110">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="O110">
-        <v>1985</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
@@ -5692,10 +5657,10 @@
         <v>638413.24106328096</v>
       </c>
       <c r="N111">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="O111">
-        <v>1986</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
@@ -5736,10 +5701,10 @@
         <v>628807.70593987498</v>
       </c>
       <c r="N112">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="O112">
-        <v>1987</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
@@ -5780,10 +5745,10 @@
         <v>636126.37466429896</v>
       </c>
       <c r="N113">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="O113">
-        <v>1988</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
@@ -5824,10 +5789,10 @@
         <v>624664.71257902996</v>
       </c>
       <c r="N114">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="O114">
-        <v>1989</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
@@ -5868,10 +5833,10 @@
         <v>626662.80963279097</v>
       </c>
       <c r="N115">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="O115">
-        <v>1990</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
@@ -5912,10 +5877,10 @@
         <v>639130.56199565204</v>
       </c>
       <c r="N116">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="O116">
-        <v>1991</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
@@ -5956,10 +5921,10 @@
         <v>641492.72481258505</v>
       </c>
       <c r="N117">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="O117">
-        <v>1992</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
@@ -6000,10 +5965,10 @@
         <v>647042.449249445</v>
       </c>
       <c r="N118">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="O118">
-        <v>1993</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
@@ -6044,10 +6009,10 @@
         <v>655956.48643901595</v>
       </c>
       <c r="N119">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="O119">
-        <v>1994</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
@@ -6088,10 +6053,10 @@
         <v>639850.05665493896</v>
       </c>
       <c r="N120">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="O120">
-        <v>1995</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
@@ -6132,10 +6097,10 @@
         <v>658277.62617324805</v>
       </c>
       <c r="N121">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="O121">
-        <v>1996</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
@@ -6176,10 +6141,10 @@
         <v>652677.81883644999</v>
       </c>
       <c r="N122">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="O122">
-        <v>1997</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
@@ -6220,10 +6185,10 @@
         <v>660448.56679253106</v>
       </c>
       <c r="N123">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="O123">
-        <v>1998</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
@@ -6264,10 +6229,10 @@
         <v>668696.619277208</v>
       </c>
       <c r="N124">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="O124">
-        <v>1999</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
@@ -6308,10 +6273,10 @@
         <v>678792.97854562395</v>
       </c>
       <c r="N125">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="O125">
-        <v>2000</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
@@ -6352,10 +6317,10 @@
         <v>684827.30767970299</v>
       </c>
       <c r="N126">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O126">
-        <v>2001</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
@@ -6396,10 +6361,10 @@
         <v>678830.64873632102</v>
       </c>
       <c r="N127">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="O127">
-        <v>2002</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
@@ -6440,10 +6405,10 @@
         <v>689168.10585742898</v>
       </c>
       <c r="N128">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="O128">
-        <v>2003</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.25">
@@ -6484,10 +6449,10 @@
         <v>680868.75882341503</v>
       </c>
       <c r="N129">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="O129">
-        <v>2004</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.25">
@@ -6528,10 +6493,10 @@
         <v>696151.96185475495</v>
       </c>
       <c r="N130">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="O130">
-        <v>2005</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.25">
@@ -6572,10 +6537,10 @@
         <v>693096.63556618895</v>
       </c>
       <c r="N131">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="O131">
-        <v>2006</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
@@ -6616,10 +6581,10 @@
         <v>688844.50927343802</v>
       </c>
       <c r="N132">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="O132">
-        <v>2007</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.25">
@@ -6660,10 +6625,10 @@
         <v>691742.49886508903</v>
       </c>
       <c r="N133">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="O133">
-        <v>2008</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
@@ -6704,10 +6669,10 @@
         <v>701582.167521102</v>
       </c>
       <c r="N134">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="O134">
-        <v>2009</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
@@ -6748,10 +6713,10 @@
         <v>709388.78701496602</v>
       </c>
       <c r="N135">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="O135">
-        <v>2010</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
@@ -6792,10 +6757,10 @@
         <v>696890.31223890802</v>
       </c>
       <c r="N136">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="O136">
-        <v>2011</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
@@ -6836,10 +6801,10 @@
         <v>710340.62104236195</v>
       </c>
       <c r="N137">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="O137">
-        <v>2012</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.25">
@@ -6880,10 +6845,10 @@
         <v>706305.47658844804</v>
       </c>
       <c r="N138">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="O138">
-        <v>2013</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.25">
@@ -6924,10 +6889,10 @@
         <v>706773.17660188104</v>
       </c>
       <c r="N139">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="O139">
-        <v>2014</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.25">
@@ -6968,10 +6933,10 @@
         <v>702579.88102730596</v>
       </c>
       <c r="N140">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="O140">
-        <v>2015</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
@@ -7012,10 +6977,10 @@
         <v>712997.76116455905</v>
       </c>
       <c r="N141">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O141">
-        <v>2016</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
@@ -7056,10 +7021,10 @@
         <v>710228.02877330699</v>
       </c>
       <c r="N142">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="O142">
-        <v>2017</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.25">
@@ -7100,10 +7065,10 @@
         <v>703581.06303391198</v>
       </c>
       <c r="N143">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="O143">
-        <v>2018</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.25">
@@ -7144,10 +7109,10 @@
         <v>718170.46638848598</v>
       </c>
       <c r="N144">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="O144">
-        <v>2019</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.25">
@@ -7188,10 +7153,10 @@
         <v>711752.62720252504</v>
       </c>
       <c r="N145">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="O145">
-        <v>2020</v>
+        <v>2014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>